<commit_message>
More convergence testing; started to add an Hv with <lm|V(x,y,z)|l'm'> pre-calculated
</commit_message>
<xml_diff>
--- a/Testing/EigenvalueCheck/Eigenvalues.xlsx
+++ b/Testing/EigenvalueCheck/Eigenvalues.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="137">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -387,6 +387,57 @@
   <si>
     <t>Ideal: E = hbar *w * (2k+l+3/2) = hbar * w * (n+3/2)</t>
   </si>
+  <si>
+    <t>bohr =</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>Edge for Alavi/SPC/E potential:</t>
+  </si>
+  <si>
+    <t>bohr</t>
+  </si>
+  <si>
+    <t>V(edge) =</t>
+  </si>
+  <si>
+    <t>V(mid) =</t>
+  </si>
+  <si>
+    <t>cm-1</t>
+  </si>
+  <si>
+    <t>Based off of Xu_2008_sIISmallCageH2WaterPES.pdf</t>
+  </si>
+  <si>
+    <t>(NIST)</t>
+  </si>
+  <si>
+    <t>kJ/mol =</t>
+  </si>
+  <si>
+    <t>cm^-1</t>
+  </si>
+  <si>
+    <t>(http://users.mccammon.ucsd.edu/~dzhang/energy-unit-conv-table.html)</t>
+  </si>
+  <si>
+    <t>w=</t>
+  </si>
+  <si>
+    <t>/ps</t>
+  </si>
+  <si>
+    <t>based on w = sqrt(2V/mr^2)</t>
+  </si>
+  <si>
+    <t>Edge=</t>
+  </si>
 </sst>
 </file>
 
@@ -457,7 +508,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="265">
+  <cellStyleXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -723,8 +774,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -744,8 +797,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="265">
+  <cellStyles count="267">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -878,6 +937,7 @@
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1010,6 +1070,7 @@
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -58301,78 +58362,456 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B13"/>
+  <dimension ref="A3:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8">
+        <v>-550</v>
+      </c>
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="6">
+        <f>B8/$B$20</f>
+        <v>-6.5794982833490838</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="6">
+        <f>SQRT(2*ABS($B$9)/$B$13/$B$6/$B$6)</f>
+        <v>2.555075975549526</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="16"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B6">
+      <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B7">
+      <c r="B13">
         <v>2.0156500639999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8">
+      <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B9">
+      <c r="B15">
         <v>3.14159265358979</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B10">
+      <c r="B16">
         <v>5.7276563844481799E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B11">
+      <c r="B17">
         <v>6.3507785700200006E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="6">
+        <v>5.2917720999999999E-11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="6">
+        <f>B18*1000000000</f>
+        <v>5.2917721000000001E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="6">
+        <v>83.593000000000004</v>
+      </c>
+      <c r="C20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>81</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B22" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <f>$B$17*$B$10*(A23+1.5)</f>
+        <v>0.24340082625439316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:B49" si="0">$B$17*$B$10*(A24+1.5)</f>
+        <v>0.40566804375732191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.56793526126025073</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.73020247876317945</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.89246969626610828</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1.054736913769037</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1.2170041312719657</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1.3792713487748947</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1.5415385662778234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>1.7038057837807521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>1.8660730012836808</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>2.0283402187866097</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>2.1906074362895382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>2.3528746537924672</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>2.5151418712953961</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>2.6774090887983246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>2.8396763063012536</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>3.0019435238041825</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>3.164210741307111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>3.3264779588100399</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>3.4887451763129684</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>3.6510123938158974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>3.8132796113188263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>3.9755468288217548</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>4.1378140463246833</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>4.3000812638276127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>26</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>4.4623484813305412</v>
       </c>
     </row>
   </sheetData>
@@ -58390,7 +58829,7 @@
   <dimension ref="A3:C81"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B13"/>
+      <selection activeCell="C6" sqref="C6:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Finished modifying Hv to precalculate potential, did some testing
</commit_message>
<xml_diff>
--- a/Testing/EigenvalueCheck/Eigenvalues.xlsx
+++ b/Testing/EigenvalueCheck/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23940" yWindow="1920" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="13400" yWindow="420" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,10 @@
     <sheet name="FreeRotor" sheetId="5" r:id="rId5"/>
     <sheet name="RotationlessHarmonicOscillator" sheetId="6" r:id="rId6"/>
     <sheet name="RotationlessCoulombPotential" sheetId="7" r:id="rId7"/>
-    <sheet name="TimingLanczosParallelization" sheetId="8" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="102">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -277,111 +279,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>None:</t>
-  </si>
-  <si>
-    <t>1st Loop:</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>Avg</t>
-  </si>
-  <si>
-    <t>RSD</t>
-  </si>
-  <si>
-    <t>Std Dev</t>
-  </si>
-  <si>
-    <t>95% CI, T-dist</t>
-  </si>
-  <si>
-    <t>2nd Loop:</t>
-  </si>
-  <si>
-    <t>4th Loop:</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>Toby (1000 iterations):</t>
-  </si>
-  <si>
-    <t>Mac (1000 iterations):</t>
-  </si>
-  <si>
-    <t>6th Loop:</t>
-  </si>
-  <si>
-    <t>7th Loop:</t>
-  </si>
-  <si>
-    <t>8th Loop:</t>
-  </si>
-  <si>
-    <t>None (after):</t>
-  </si>
-  <si>
-    <t>No Hv Parallelization:</t>
-  </si>
-  <si>
-    <t>Mv_5D_oneCompositeIndex</t>
-  </si>
-  <si>
-    <t>Mv_5D_oneCompositeIndex (no collapse)</t>
-  </si>
-  <si>
-    <t>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</t>
-  </si>
-  <si>
-    <t>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</t>
-  </si>
-  <si>
-    <t>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</t>
-  </si>
-  <si>
-    <t>Order of Execution:</t>
-  </si>
-  <si>
-    <t>diagMv_5D_oneCompositeIndex</t>
-  </si>
-  <si>
-    <t>calc_ulm</t>
-  </si>
-  <si>
-    <t>reshuffleIndices_5D_oneCompositeIndex</t>
-  </si>
-  <si>
-    <t>Hv_5D_oneCompositeIndex</t>
-  </si>
-  <si>
-    <t>Too long! Estimate is 2266s NOTE: this may not be a fair assessment as na and nb are only 2 and l_max =0</t>
-  </si>
-  <si>
-    <t>Need to check Cartesian grid generator with larger nx,ny,nz</t>
-  </si>
-  <si>
-    <t>Need to check calc_ulm, diagMv with larger na,nb, lmax</t>
-  </si>
-  <si>
-    <t>Need to check Hv_prep with larger system sizes</t>
-  </si>
-  <si>
-    <t>Need to check eliminating excess uec loops in lanczos algorithm</t>
-  </si>
-  <si>
-    <t>Reactivate Coulomb Calc (with Vv parallelized)</t>
-  </si>
-  <si>
     <t>V(r) = 1/2 * m * w^2 r^2</t>
   </si>
   <si>
@@ -443,9 +340,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -777,7 +673,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -792,16 +688,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="267">
@@ -1078,552 +972,150 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Effect of Lanczos Loop Parallelization</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="1"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>TimingLanczosParallelization!$J$14:$J$22</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
-                  <c:pt idx="0">
-                    <c:v>0.0417070485706302</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.15960095137594</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.115092669407768</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.0480253361511355</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.00912933227292609</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.0549375410519272</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.124112005810021</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.0259357984507788</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.0732697357397158</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>TimingLanczosParallelization!$J$14:$J$22</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
-                  <c:pt idx="0">
-                    <c:v>0.0417070485706302</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.15960095137594</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.115092669407768</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.0480253361511355</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.00912933227292609</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.0549375410519272</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.124112005810021</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.0259357984507788</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.0732697357397158</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>TimingLanczosParallelization!$B$14:$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>None:</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1st Loop:</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2nd Loop:</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4th Loop:</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6th Loop:</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7th Loop:</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8th Loop:</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>None (after):</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>No Hv Parallelization:</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TimingLanczosParallelization!$G$14:$G$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.871</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.02125</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.99875</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.90975</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.893750000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.96</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.9785</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.9125</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.04725</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="505484312"/>
-        <c:axId val="505490936"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="505484312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="505490936"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="505490936"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="4.9"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Execution Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="505484312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Effect of Collapse Directive on Vv_5D_Composite</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Index</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="1"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>(TimingLanczosParallelization!$J$23,TimingLanczosParallelization!$J$26:$J$27)</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0.0616688792220049</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0700921306050633</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0328296241330902</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>(TimingLanczosParallelization!$J$23,TimingLanczosParallelization!$J$26:$J$27)</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0.0616688792220049</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0700921306050633</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.0328296241330902</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>(TimingLanczosParallelization!$B$23,TimingLanczosParallelization!$B$26:$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(TimingLanczosParallelization!$G$23,TimingLanczosParallelization!$G$26:$G$27)</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3.212</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.4185</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.2905</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="497086456"/>
-        <c:axId val="497089368"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="497086456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497089368"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="497089368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Execution Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497086456"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="TimingLanczosParallelization"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>None:</v>
+          </cell>
+          <cell r="G14">
+            <v>5.8709999999999996</v>
+          </cell>
+          <cell r="J14">
+            <v>4.1707048570630241E-2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>1st Loop:</v>
+          </cell>
+          <cell r="G15">
+            <v>6.0212500000000002</v>
+          </cell>
+          <cell r="J15">
+            <v>0.15960095137594044</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>2nd Loop:</v>
+          </cell>
+          <cell r="G16">
+            <v>5.9987500000000002</v>
+          </cell>
+          <cell r="J16">
+            <v>0.11509266940776765</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>4th Loop:</v>
+          </cell>
+          <cell r="G17">
+            <v>5.9097500000000007</v>
+          </cell>
+          <cell r="J17">
+            <v>4.8025336151135523E-2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>6th Loop:</v>
+          </cell>
+          <cell r="G18">
+            <v>5.8937500000000007</v>
+          </cell>
+          <cell r="J18">
+            <v>9.1293322729260884E-3</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>7th Loop:</v>
+          </cell>
+          <cell r="G19">
+            <v>5.96</v>
+          </cell>
+          <cell r="J19">
+            <v>5.4937541051927184E-2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>8th Loop:</v>
+          </cell>
+          <cell r="G20">
+            <v>5.9785000000000004</v>
+          </cell>
+          <cell r="J20">
+            <v>0.12411200581002095</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>None (after):</v>
+          </cell>
+          <cell r="G21">
+            <v>5.9124999999999996</v>
+          </cell>
+          <cell r="J21">
+            <v>2.5935798450778775E-2</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>No Hv Parallelization:</v>
+          </cell>
+          <cell r="G22">
+            <v>5.04725</v>
+          </cell>
+          <cell r="J22">
+            <v>7.3269735739715805E-2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</v>
+          </cell>
+          <cell r="G23">
+            <v>3.2119999999999997</v>
+          </cell>
+          <cell r="J23">
+            <v>6.1668879222004876E-2</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</v>
+          </cell>
+          <cell r="G26">
+            <v>3.4185000000000003</v>
+          </cell>
+          <cell r="J26">
+            <v>7.0092130605063308E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</v>
+          </cell>
+          <cell r="G27">
+            <v>3.2905000000000002</v>
+          </cell>
+          <cell r="J27">
+            <v>3.2829624133090242E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58364,7 +57856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -58372,43 +57864,43 @@
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="15" t="s">
-        <v>123</v>
+      <c r="A5" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="15" t="s">
-        <v>136</v>
+      <c r="A6" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="B6" s="6">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="15" t="s">
-        <v>125</v>
+      <c r="A7" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -58418,19 +57910,19 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="15" t="s">
-        <v>126</v>
+      <c r="A8" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="B8">
         <v>-550</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="16" t="s">
-        <v>121</v>
+      <c r="A9" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="B9" s="6">
         <f>B8/$B$20</f>
@@ -58441,26 +57933,26 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="16" t="s">
-        <v>133</v>
+      <c r="A10" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="B10" s="6">
         <f>SQRT(2*ABS($B$9)/$B$13/$B$6/$B$6)</f>
         <v>2.555075975549526</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="16"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B12">
@@ -58471,7 +57963,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>75</v>
       </c>
       <c r="B13">
@@ -58482,7 +57974,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B14">
@@ -58493,7 +57985,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B15">
@@ -58501,7 +57993,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B16">
@@ -58509,7 +58001,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B17">
@@ -58520,8 +58012,8 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="15" t="s">
-        <v>120</v>
+      <c r="A18" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="6">
         <v>5.2917720999999999E-11</v>
@@ -58530,37 +58022,37 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="16" t="s">
-        <v>121</v>
+      <c r="A19" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="B19" s="6">
         <f>B18*1000000000</f>
         <v>5.2917721000000001E-2</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="16" t="s">
-        <v>130</v>
+      <c r="A20" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="B20" s="6">
         <v>83.593000000000004</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="16"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:4">
@@ -58828,8 +58320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C81"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59534,969 +59026,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
-  <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="12">
-        <v>7.5880000000000001</v>
-      </c>
-      <c r="C3" s="12">
-        <v>6.3140000000000001</v>
-      </c>
-      <c r="D3">
-        <v>6.2160000000000002</v>
-      </c>
-      <c r="F3" s="12">
-        <f>AVERAGE(B3:D3)</f>
-        <v>6.7060000000000004</v>
-      </c>
-      <c r="G3" s="12">
-        <f>STDEV(B3:D3)</f>
-        <v>0.76540446823885211</v>
-      </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="0">G3/F3</f>
-        <v>0.11413726039947093</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I10" si="1">_xlfn.T.INV.2T(0.05, COUNT(B3:E3)-1)*G3/SQRT(COUNT(B3:E3))</f>
-        <v>1.9013701042943409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="12">
-        <v>8.0449999999999999</v>
-      </c>
-      <c r="C4" s="12">
-        <v>10.086</v>
-      </c>
-      <c r="D4" s="12">
-        <v>9.3800000000000008</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12">
-        <f>AVERAGE(B4:D4)</f>
-        <v>9.1703333333333337</v>
-      </c>
-      <c r="G4" s="12">
-        <f>STDEV(B4:D4)</f>
-        <v>1.0365280185954135</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="0"/>
-        <v>0.11303057161812513</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>2.574878340278715</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5">
-        <v>7.3360000000000003</v>
-      </c>
-      <c r="C5">
-        <v>7.7709999999999999</v>
-      </c>
-      <c r="D5">
-        <v>6.6289999999999996</v>
-      </c>
-      <c r="E5">
-        <v>8.3059999999999992</v>
-      </c>
-      <c r="F5" s="12">
-        <f>AVERAGE(B5:E5)</f>
-        <v>7.5104999999999986</v>
-      </c>
-      <c r="G5" s="12">
-        <f>STDEV(B5:E5)</f>
-        <v>0.70903055881487442</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" ref="H5:H7" si="2">G5/F5</f>
-        <v>9.4405240505275892E-2</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>1.1282258411168204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6">
-        <v>6.6529999999999996</v>
-      </c>
-      <c r="C6">
-        <v>6.8810000000000002</v>
-      </c>
-      <c r="D6">
-        <v>9.1470000000000002</v>
-      </c>
-      <c r="E6">
-        <v>5.3940000000000001</v>
-      </c>
-      <c r="F6" s="12">
-        <f>AVERAGE(B6:E6)</f>
-        <v>7.0187499999999989</v>
-      </c>
-      <c r="G6" s="12">
-        <f>STDEV(B6:E6)</f>
-        <v>1.5622642488815248</v>
-      </c>
-      <c r="H6" s="13">
-        <f t="shared" si="2"/>
-        <v>0.22258439877207836</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>2.485911043364919</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="F7" s="12" t="e">
-        <f t="shared" ref="F7:F10" si="3">AVERAGE(B7:D7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="12" t="e">
-        <f t="shared" ref="G7:G10" si="4">STDEV(B7:D7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="F8" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="12" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="13" t="e">
-        <f t="shared" ref="H8:H10" si="5">G8/F8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="F9" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="12" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="13" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="F10" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G10" s="12" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="13" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="12">
-        <v>5.8490000000000002</v>
-      </c>
-      <c r="D14" s="12">
-        <v>5.9</v>
-      </c>
-      <c r="E14" s="12">
-        <v>5.8639999999999999</v>
-      </c>
-      <c r="F14" s="12">
-        <v>5.8470000000000004</v>
-      </c>
-      <c r="G14" s="12">
-        <f>AVERAGE(C14:E14)</f>
-        <v>5.8709999999999996</v>
-      </c>
-      <c r="H14" s="12">
-        <f>STDEV(C14:E14)</f>
-        <v>2.6210684844162443E-2</v>
-      </c>
-      <c r="I14" s="13">
-        <f t="shared" ref="I14:I21" si="6">H14/G14</f>
-        <v>4.4644327787706425E-3</v>
-      </c>
-      <c r="J14">
-        <f t="shared" ref="J14:J21" si="7">_xlfn.T.INV.2T(0.05, COUNT(C14:F14)-1)*H14/SQRT(COUNT(C14:F14))</f>
-        <v>4.1707048570630241E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="12">
-        <v>6.1559999999999997</v>
-      </c>
-      <c r="D15" s="12">
-        <v>6.0369999999999999</v>
-      </c>
-      <c r="E15" s="12">
-        <v>5.931</v>
-      </c>
-      <c r="F15" s="12">
-        <v>5.9610000000000003</v>
-      </c>
-      <c r="G15" s="12">
-        <f t="shared" ref="G15:G21" si="8">AVERAGE(C15:F15)</f>
-        <v>6.0212500000000002</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" ref="H15:H21" si="9">STDEV(C15:F15)</f>
-        <v>0.1003007976040069</v>
-      </c>
-      <c r="I15" s="13">
-        <f t="shared" si="6"/>
-        <v>1.6657803214283895E-2</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="7"/>
-        <v>0.15960095137594044</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="12">
-        <v>5.8979999999999997</v>
-      </c>
-      <c r="D16" s="12">
-        <v>6.0620000000000003</v>
-      </c>
-      <c r="E16" s="12">
-        <v>5.9969999999999999</v>
-      </c>
-      <c r="F16" s="12">
-        <v>6.0380000000000003</v>
-      </c>
-      <c r="G16" s="12">
-        <f t="shared" si="8"/>
-        <v>5.9987500000000002</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="9"/>
-        <v>7.2329685007840122E-2</v>
-      </c>
-      <c r="I16" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2057459472030026E-2</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="7"/>
-        <v>0.11509266940776765</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="12">
-        <v>5.95</v>
-      </c>
-      <c r="D17" s="12">
-        <v>5.915</v>
-      </c>
-      <c r="E17" s="12">
-        <v>5.8920000000000003</v>
-      </c>
-      <c r="F17" s="12">
-        <v>5.8819999999999997</v>
-      </c>
-      <c r="G17" s="12">
-        <f t="shared" si="8"/>
-        <v>5.9097500000000007</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="9"/>
-        <v>3.018139603574814E-2</v>
-      </c>
-      <c r="I17" s="13">
-        <f t="shared" si="6"/>
-        <v>5.1070512349504016E-3</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="7"/>
-        <v>4.8025336151135523E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="12">
-        <v>5.891</v>
-      </c>
-      <c r="D18" s="12">
-        <v>5.8890000000000002</v>
-      </c>
-      <c r="E18" s="12">
-        <v>5.8929999999999998</v>
-      </c>
-      <c r="F18" s="12">
-        <v>5.9020000000000001</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" si="8"/>
-        <v>5.8937500000000007</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="9"/>
-        <v>5.7373048260195084E-3</v>
-      </c>
-      <c r="I18" s="13">
-        <f t="shared" si="6"/>
-        <v>9.7345574990786977E-4</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="7"/>
-        <v>9.1293322729260884E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="12">
-        <v>5.9820000000000002</v>
-      </c>
-      <c r="D19" s="12">
-        <v>5.9880000000000004</v>
-      </c>
-      <c r="E19" s="12">
-        <v>5.9580000000000002</v>
-      </c>
-      <c r="F19" s="12">
-        <v>5.9119999999999999</v>
-      </c>
-      <c r="G19" s="12">
-        <f t="shared" si="8"/>
-        <v>5.96</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="9"/>
-        <v>3.4525353003264328E-2</v>
-      </c>
-      <c r="I19" s="13">
-        <f t="shared" si="6"/>
-        <v>5.7928444636349543E-3</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="7"/>
-        <v>5.4937541051927184E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="12">
-        <v>5.984</v>
-      </c>
-      <c r="D20" s="12">
-        <v>5.952</v>
-      </c>
-      <c r="E20" s="12">
-        <v>5.8959999999999999</v>
-      </c>
-      <c r="F20" s="12">
-        <v>6.0819999999999999</v>
-      </c>
-      <c r="G20" s="12">
-        <f t="shared" si="8"/>
-        <v>5.9785000000000004</v>
-      </c>
-      <c r="H20" s="12">
-        <f t="shared" si="9"/>
-        <v>7.7997863218595045E-2</v>
-      </c>
-      <c r="I20" s="13">
-        <f t="shared" si="6"/>
-        <v>1.3046393446281683E-2</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="7"/>
-        <v>0.12411200581002095</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="12">
-        <v>5.931</v>
-      </c>
-      <c r="D21" s="12">
-        <v>5.92</v>
-      </c>
-      <c r="E21" s="12">
-        <v>5.8940000000000001</v>
-      </c>
-      <c r="F21" s="12">
-        <v>5.9050000000000002</v>
-      </c>
-      <c r="G21" s="12">
-        <f t="shared" si="8"/>
-        <v>5.9124999999999996</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="9"/>
-        <v>1.6299284237863455E-2</v>
-      </c>
-      <c r="I21" s="13">
-        <f t="shared" si="6"/>
-        <v>2.7567499768056587E-3</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="7"/>
-        <v>2.5935798450778775E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="12">
-        <v>4.9969999999999999</v>
-      </c>
-      <c r="D22" s="12">
-        <v>5.0529999999999999</v>
-      </c>
-      <c r="E22" s="12">
-        <v>5.032</v>
-      </c>
-      <c r="F22" s="12">
-        <v>5.1070000000000002</v>
-      </c>
-      <c r="G22" s="12">
-        <f t="shared" ref="G22:G28" si="10">AVERAGE(C22:F22)</f>
-        <v>5.04725</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" ref="H22:H28" si="11">STDEV(C22:F22)</f>
-        <v>4.6046172479371303E-2</v>
-      </c>
-      <c r="I22" s="13">
-        <f t="shared" ref="I22:I28" si="12">H22/G22</f>
-        <v>9.1230219385549163E-3</v>
-      </c>
-      <c r="J22">
-        <f t="shared" ref="J22:J28" si="13">_xlfn.T.INV.2T(0.05, COUNT(C22:F22)-1)*H22/SQRT(COUNT(C22:F22))</f>
-        <v>7.3269735739715805E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="12">
-        <v>3.16</v>
-      </c>
-      <c r="D23" s="12">
-        <v>3.2120000000000002</v>
-      </c>
-      <c r="E23" s="12">
-        <v>3.2530000000000001</v>
-      </c>
-      <c r="F23" s="12">
-        <v>3.2229999999999999</v>
-      </c>
-      <c r="G23" s="12">
-        <f t="shared" si="10"/>
-        <v>3.2119999999999997</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" si="11"/>
-        <v>3.8755644750152168E-2</v>
-      </c>
-      <c r="I23" s="13">
-        <f t="shared" si="12"/>
-        <v>1.2065891889835669E-2</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="13"/>
-        <v>6.1668879222004876E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="12">
-        <v>5.8170000000000002</v>
-      </c>
-      <c r="D24" s="12">
-        <v>5.8179999999999996</v>
-      </c>
-      <c r="E24" s="12">
-        <v>5.8479999999999999</v>
-      </c>
-      <c r="F24" s="12">
-        <v>5.8040000000000003</v>
-      </c>
-      <c r="G24" s="12">
-        <f t="shared" si="10"/>
-        <v>5.8217499999999998</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="11"/>
-        <v>1.8625699092025019E-2</v>
-      </c>
-      <c r="I24" s="13">
-        <f t="shared" si="12"/>
-        <v>3.1993299423755776E-3</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="13"/>
-        <v>2.9637643629370578E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="12">
-        <v>5.9909999999999997</v>
-      </c>
-      <c r="D25" s="12">
-        <v>5.9640000000000004</v>
-      </c>
-      <c r="E25" s="12">
-        <v>5.9630000000000001</v>
-      </c>
-      <c r="F25" s="12">
-        <v>6.024</v>
-      </c>
-      <c r="G25" s="12">
-        <f t="shared" si="10"/>
-        <v>5.9855</v>
-      </c>
-      <c r="H25" s="12">
-        <f t="shared" si="11"/>
-        <v>2.8757607689096677E-2</v>
-      </c>
-      <c r="I25" s="13">
-        <f t="shared" si="12"/>
-        <v>4.8045456000495659E-3</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="13"/>
-        <v>4.5759771169482051E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="12">
-        <v>3.403</v>
-      </c>
-      <c r="D26" s="12">
-        <v>3.3650000000000002</v>
-      </c>
-      <c r="E26" s="12">
-        <v>3.4660000000000002</v>
-      </c>
-      <c r="F26" s="12">
-        <v>3.44</v>
-      </c>
-      <c r="G26" s="12">
-        <f t="shared" si="10"/>
-        <v>3.4185000000000003</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="11"/>
-        <v>4.4049214900305896E-2</v>
-      </c>
-      <c r="I26" s="13">
-        <f t="shared" si="12"/>
-        <v>1.2885538949921279E-2</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="13"/>
-        <v>7.0092130605063308E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="12">
-        <v>3.3109999999999999</v>
-      </c>
-      <c r="D27" s="12">
-        <v>3.262</v>
-      </c>
-      <c r="E27" s="12">
-        <v>3.2919999999999998</v>
-      </c>
-      <c r="F27" s="12">
-        <v>3.2970000000000002</v>
-      </c>
-      <c r="G27" s="12">
-        <f t="shared" si="10"/>
-        <v>3.2905000000000002</v>
-      </c>
-      <c r="H27" s="12">
-        <f t="shared" si="11"/>
-        <v>2.0631690833925031E-2</v>
-      </c>
-      <c r="I27" s="13">
-        <f t="shared" si="12"/>
-        <v>6.2700777492554413E-3</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="13"/>
-        <v>3.2829624133090242E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28">
-        <v>14</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="12">
-        <v>5.8310000000000004</v>
-      </c>
-      <c r="D28" s="12">
-        <v>5.7990000000000004</v>
-      </c>
-      <c r="E28" s="12">
-        <v>5.8109999999999999</v>
-      </c>
-      <c r="F28" s="12">
-        <v>5.8860000000000001</v>
-      </c>
-      <c r="G28" s="12">
-        <f t="shared" si="10"/>
-        <v>5.8317500000000004</v>
-      </c>
-      <c r="H28" s="12">
-        <f t="shared" si="11"/>
-        <v>3.8499999999999958E-2</v>
-      </c>
-      <c r="I28" s="13">
-        <f t="shared" si="12"/>
-        <v>6.6017919149483351E-3</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="13"/>
-        <v>6.1262091376711333E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
-        <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="12">
-        <v>6.1120000000000001</v>
-      </c>
-      <c r="D30" s="12">
-        <v>6.1550000000000002</v>
-      </c>
-      <c r="E30" s="12">
-        <v>6.5460000000000003</v>
-      </c>
-      <c r="F30" s="12">
-        <v>6.2110000000000003</v>
-      </c>
-      <c r="G30" s="12">
-        <f t="shared" ref="G30:G32" si="14">AVERAGE(C30:F30)</f>
-        <v>6.2560000000000002</v>
-      </c>
-      <c r="H30" s="12">
-        <f t="shared" ref="H30:H32" si="15">STDEV(C30:F30)</f>
-        <v>0.19753649451852354</v>
-      </c>
-      <c r="I30" s="13">
-        <f t="shared" ref="I30:I32" si="16">H30/G30</f>
-        <v>3.1575526617411052E-2</v>
-      </c>
-      <c r="J30">
-        <f t="shared" ref="J30:J32" si="17">_xlfn.T.INV.2T(0.05, COUNT(C30:F30)-1)*H30/SQRT(COUNT(C30:F30))</f>
-        <v>0.31432464356958545</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
-        <v>17</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="12">
-        <v>5.9320000000000004</v>
-      </c>
-      <c r="D31" s="12">
-        <v>5.8959999999999999</v>
-      </c>
-      <c r="E31" s="12">
-        <v>5.9020000000000001</v>
-      </c>
-      <c r="F31" s="12">
-        <v>5.9059999999999997</v>
-      </c>
-      <c r="G31" s="12">
-        <f t="shared" si="14"/>
-        <v>5.9089999999999998</v>
-      </c>
-      <c r="H31" s="12">
-        <f t="shared" si="15"/>
-        <v>1.5874507866387753E-2</v>
-      </c>
-      <c r="I31" s="13">
-        <f t="shared" si="16"/>
-        <v>2.6864965081042059E-3</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="17"/>
-        <v>2.5259884453791438E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="12">
-        <v>6.7910000000000004</v>
-      </c>
-      <c r="D32" s="12">
-        <v>6.7350000000000003</v>
-      </c>
-      <c r="E32" s="12">
-        <v>6.6689999999999996</v>
-      </c>
-      <c r="F32" s="12">
-        <v>6.7469999999999999</v>
-      </c>
-      <c r="G32" s="12">
-        <f t="shared" si="14"/>
-        <v>6.7355</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="15"/>
-        <v>5.044799302251806E-2</v>
-      </c>
-      <c r="I32" s="13">
-        <f t="shared" si="16"/>
-        <v>7.4898660860393523E-3</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="17"/>
-        <v>8.0274014501745469E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a symmeterizer to NoQuad Hv and did a test on Toby, I am getting close to Bacics results.
</commit_message>
<xml_diff>
--- a/Testing/EigenvalueCheck/Eigenvalues.xlsx
+++ b/Testing/EigenvalueCheck/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="420" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="15780" yWindow="740" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,6 @@
     <sheet name="RotationlessHarmonicOscillator" sheetId="6" r:id="rId6"/>
     <sheet name="RotationlessCoulombPotential" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -340,8 +337,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -404,7 +402,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="267">
+  <cellStyleXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -672,8 +670,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -697,8 +709,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="267">
+  <cellStyles count="281">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -832,6 +845,13 @@
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -965,157 +985,18 @@
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TimingLanczosParallelization"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>None:</v>
-          </cell>
-          <cell r="G14">
-            <v>5.8709999999999996</v>
-          </cell>
-          <cell r="J14">
-            <v>4.1707048570630241E-2</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>1st Loop:</v>
-          </cell>
-          <cell r="G15">
-            <v>6.0212500000000002</v>
-          </cell>
-          <cell r="J15">
-            <v>0.15960095137594044</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>2nd Loop:</v>
-          </cell>
-          <cell r="G16">
-            <v>5.9987500000000002</v>
-          </cell>
-          <cell r="J16">
-            <v>0.11509266940776765</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>4th Loop:</v>
-          </cell>
-          <cell r="G17">
-            <v>5.9097500000000007</v>
-          </cell>
-          <cell r="J17">
-            <v>4.8025336151135523E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>6th Loop:</v>
-          </cell>
-          <cell r="G18">
-            <v>5.8937500000000007</v>
-          </cell>
-          <cell r="J18">
-            <v>9.1293322729260884E-3</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>7th Loop:</v>
-          </cell>
-          <cell r="G19">
-            <v>5.96</v>
-          </cell>
-          <cell r="J19">
-            <v>5.4937541051927184E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>8th Loop:</v>
-          </cell>
-          <cell r="G20">
-            <v>5.9785000000000004</v>
-          </cell>
-          <cell r="J20">
-            <v>0.12411200581002095</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>None (after):</v>
-          </cell>
-          <cell r="G21">
-            <v>5.9124999999999996</v>
-          </cell>
-          <cell r="J21">
-            <v>2.5935798450778775E-2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>No Hv Parallelization:</v>
-          </cell>
-          <cell r="G22">
-            <v>5.04725</v>
-          </cell>
-          <cell r="J22">
-            <v>7.3269735739715805E-2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</v>
-          </cell>
-          <cell r="G23">
-            <v>3.2119999999999997</v>
-          </cell>
-          <cell r="J23">
-            <v>6.1668879222004876E-2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</v>
-          </cell>
-          <cell r="G26">
-            <v>3.4185000000000003</v>
-          </cell>
-          <cell r="J26">
-            <v>7.0092130605063308E-2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</v>
-          </cell>
-          <cell r="G27">
-            <v>3.2905000000000002</v>
-          </cell>
-          <cell r="J27">
-            <v>3.2829624133090242E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57854,13 +57735,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D49"/>
+  <dimension ref="A3:F49"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -58000,7 +57884,7 @@
         <v>5.7276563844481799E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17" s="12" t="s">
         <v>79</v>
       </c>
@@ -58011,7 +57895,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18" s="12" t="s">
         <v>85</v>
       </c>
@@ -58024,8 +57908,15 @@
       <c r="D18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>3.8</v>
+      </c>
+      <c r="F18" s="15">
+        <f>E18*B19*2</f>
+        <v>0.40217467959999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="13" t="s">
         <v>86</v>
       </c>
@@ -58037,7 +57928,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20" s="13" t="s">
         <v>95</v>
       </c>
@@ -58051,11 +57942,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21" s="13"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -58063,7 +57954,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>0</v>
       </c>
@@ -58072,7 +57963,7 @@
         <v>0.24340082625439316</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>1</v>
       </c>
@@ -58081,7 +57972,7 @@
         <v>0.40566804375732191</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>2</v>
       </c>
@@ -58090,7 +57981,7 @@
         <v>0.56793526126025073</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>3</v>
       </c>
@@ -58099,7 +57990,7 @@
         <v>0.73020247876317945</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>4</v>
       </c>
@@ -58108,7 +57999,7 @@
         <v>0.89246969626610828</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>5</v>
       </c>
@@ -58117,7 +58008,7 @@
         <v>1.054736913769037</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>6</v>
       </c>
@@ -58126,7 +58017,7 @@
         <v>1.2170041312719657</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>7</v>
       </c>
@@ -58135,7 +58026,7 @@
         <v>1.3792713487748947</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>8</v>
       </c>
@@ -58144,7 +58035,7 @@
         <v>1.5415385662778234</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>9</v>
       </c>
@@ -58308,6 +58199,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>